<commit_message>
Added Payment Screen flow
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData.xlsx
+++ b/src/test/resources/TestData/InputData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16387" windowHeight="8187" tabRatio="500" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="SpotCode_Success" sheetId="2" r:id="rId1"/>
@@ -13,6 +13,12 @@
     <sheet name="Login_Success" sheetId="1" r:id="rId4"/>
     <sheet name="Login_Failure" sheetId="4" r:id="rId5"/>
     <sheet name="LoginBlank_Failure" sheetId="8" r:id="rId6"/>
+    <sheet name="SpotNo_Success" sheetId="9" r:id="rId7"/>
+    <sheet name="SpotNo_Failure" sheetId="10" r:id="rId8"/>
+    <sheet name="EmptySpotNo_Failure" sheetId="11" r:id="rId9"/>
+    <sheet name="Payment_Success" sheetId="12" r:id="rId10"/>
+    <sheet name="PaymentBlank_Failure" sheetId="13" r:id="rId11"/>
+    <sheet name="PaymentTip_Failure" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Password</t>
   </si>
@@ -41,9 +47,6 @@
     <t>Spot Code</t>
   </si>
   <si>
-    <t>PAI11MA</t>
-  </si>
-  <si>
     <t>empty_Code</t>
   </si>
   <si>
@@ -66,13 +69,64 @@
   </si>
   <si>
     <t>empty_UserName, empty_Password</t>
+  </si>
+  <si>
+    <t>Spot Number</t>
+  </si>
+  <si>
+    <t>Error_Keys</t>
+  </si>
+  <si>
+    <t>empty_SpotNumber</t>
+  </si>
+  <si>
+    <t>%#@</t>
+  </si>
+  <si>
+    <t>invalid_SpotNumber</t>
+  </si>
+  <si>
+    <t>PAI11CU</t>
+  </si>
+  <si>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Expiry Date</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>12/20</t>
+  </si>
+  <si>
+    <t>4012881888818888</t>
+  </si>
+  <si>
+    <t>85284</t>
+  </si>
+  <si>
+    <t>invalid_CardDetails</t>
+  </si>
+  <si>
+    <t>invalid_TipCardDetails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -96,6 +150,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -117,11 +176,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,13 +490,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.75" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -444,8 +508,170 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="20.125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5"/>
+    <col min="5" max="5" width="16.875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.25" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5">
+        <v>999</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" style="5" customWidth="1"/>
+    <col min="2" max="3" width="13.25" style="5" customWidth="1"/>
+    <col min="4" max="5" width="9" style="5"/>
+    <col min="6" max="6" width="15.875" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="19.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -461,9 +687,9 @@
       <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -477,10 +703,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -496,9 +722,9 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -512,7 +738,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -525,17 +751,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="1002" width="14.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.125" customWidth="1"/>
+    <col min="2" max="2" width="29.75" customWidth="1"/>
+    <col min="3" max="1002" width="14.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -546,78 +772,78 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="29.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="19.375" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -632,8 +858,108 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.25" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>